<commit_message>
added map file support
</commit_message>
<xml_diff>
--- a/input/All_Automotive_PROFET.xlsx
+++ b/input/All_Automotive_PROFET.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basov\Documents\_WORK IFX\SoftProjects\xmind_dev\datafiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\basov\Documents\_WORK IFX\SoftProjects\product_selection_guide_builder\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
+    <workbookView minimized="1" xWindow="240" yWindow="12" windowWidth="16092" windowHeight="9660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -2889,11 +2889,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:U177"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J45" sqref="J45"/>
+      <selection sqref="A1:U1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2963,7 +2962,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>21</v>
       </c>
@@ -3028,7 +3027,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="3" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -3093,7 +3092,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="4" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>23</v>
       </c>
@@ -3158,7 +3157,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="5" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -3223,7 +3222,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="6" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>25</v>
       </c>
@@ -3288,7 +3287,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="7" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>26</v>
       </c>
@@ -3353,7 +3352,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="8" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>27</v>
       </c>
@@ -3418,7 +3417,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="9" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>28</v>
       </c>
@@ -3483,7 +3482,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="10" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>29</v>
       </c>
@@ -3548,7 +3547,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="11" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>30</v>
       </c>
@@ -3613,7 +3612,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="12" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>31</v>
       </c>
@@ -3678,7 +3677,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="13" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -3743,7 +3742,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="14" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>33</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="15" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>34</v>
       </c>
@@ -3873,7 +3872,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="16" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>35</v>
       </c>
@@ -3938,7 +3937,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="17" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>36</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="18" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>37</v>
       </c>
@@ -4068,7 +4067,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="19" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>38</v>
       </c>
@@ -4133,7 +4132,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="20" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>39</v>
       </c>
@@ -4198,7 +4197,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="21" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -4263,7 +4262,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="22" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>41</v>
       </c>
@@ -4328,7 +4327,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="23" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>42</v>
       </c>
@@ -4393,7 +4392,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="24" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>43</v>
       </c>
@@ -4458,7 +4457,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="25" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>44</v>
       </c>
@@ -4523,7 +4522,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="26" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -4588,7 +4587,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="27" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>46</v>
       </c>
@@ -4653,7 +4652,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="28" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>47</v>
       </c>
@@ -4718,7 +4717,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="29" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>48</v>
       </c>
@@ -4783,7 +4782,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="30" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>49</v>
       </c>
@@ -4848,7 +4847,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="31" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>50</v>
       </c>
@@ -4913,7 +4912,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="32" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>51</v>
       </c>
@@ -4978,7 +4977,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="33" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>52</v>
       </c>
@@ -5043,7 +5042,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="34" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>53</v>
       </c>
@@ -5108,7 +5107,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="35" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>54</v>
       </c>
@@ -5173,7 +5172,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="36" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>55</v>
       </c>
@@ -5238,7 +5237,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="37" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>56</v>
       </c>
@@ -5303,7 +5302,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="38" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>57</v>
       </c>
@@ -5368,7 +5367,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="39" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>58</v>
       </c>
@@ -5433,7 +5432,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="40" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>59</v>
       </c>
@@ -5498,7 +5497,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="41" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>60</v>
       </c>
@@ -5563,7 +5562,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="42" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>61</v>
       </c>
@@ -5823,7 +5822,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="46" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>65</v>
       </c>
@@ -5888,7 +5887,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="47" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>66</v>
       </c>
@@ -5953,7 +5952,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="48" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>67</v>
       </c>
@@ -6018,7 +6017,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="49" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>68</v>
       </c>
@@ -6083,7 +6082,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="50" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>69</v>
       </c>
@@ -6148,7 +6147,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="51" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>70</v>
       </c>
@@ -6213,7 +6212,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="52" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>71</v>
       </c>
@@ -6278,7 +6277,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="53" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>72</v>
       </c>
@@ -6343,7 +6342,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="54" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>73</v>
       </c>
@@ -6408,7 +6407,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="55" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>74</v>
       </c>
@@ -6473,7 +6472,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="56" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>75</v>
       </c>
@@ -6538,7 +6537,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="57" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>76</v>
       </c>
@@ -6603,7 +6602,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="58" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>77</v>
       </c>
@@ -6668,7 +6667,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="59" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>78</v>
       </c>
@@ -6733,7 +6732,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="60" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>79</v>
       </c>
@@ -6798,7 +6797,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="61" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>80</v>
       </c>
@@ -6863,7 +6862,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="62" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>81</v>
       </c>
@@ -6928,7 +6927,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="63" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>82</v>
       </c>
@@ -6993,7 +6992,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="64" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>83</v>
       </c>
@@ -7058,7 +7057,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="65" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>84</v>
       </c>
@@ -7123,7 +7122,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="66" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>85</v>
       </c>
@@ -7188,7 +7187,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="67" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>86</v>
       </c>
@@ -7253,7 +7252,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="68" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>87</v>
       </c>
@@ -7318,7 +7317,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="69" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>88</v>
       </c>
@@ -7383,7 +7382,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="70" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>89</v>
       </c>
@@ -7448,7 +7447,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="71" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>90</v>
       </c>
@@ -7513,7 +7512,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="72" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>91</v>
       </c>
@@ -7578,7 +7577,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="73" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>92</v>
       </c>
@@ -7643,7 +7642,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="74" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>93</v>
       </c>
@@ -7708,7 +7707,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="75" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>94</v>
       </c>
@@ -7773,7 +7772,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="76" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>95</v>
       </c>
@@ -7838,7 +7837,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="77" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>96</v>
       </c>
@@ -7903,7 +7902,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="78" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>97</v>
       </c>
@@ -7968,7 +7967,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="79" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>98</v>
       </c>
@@ -8033,7 +8032,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="80" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>99</v>
       </c>
@@ -8098,7 +8097,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="81" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>100</v>
       </c>
@@ -8163,7 +8162,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="82" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>101</v>
       </c>
@@ -8228,7 +8227,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="83" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>102</v>
       </c>
@@ -8293,7 +8292,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="84" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>103</v>
       </c>
@@ -8358,7 +8357,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="85" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>104</v>
       </c>
@@ -8423,7 +8422,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="86" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>105</v>
       </c>
@@ -8488,7 +8487,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="87" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>106</v>
       </c>
@@ -8553,7 +8552,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="88" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>107</v>
       </c>
@@ -8618,7 +8617,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="89" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>108</v>
       </c>
@@ -8683,7 +8682,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="90" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>109</v>
       </c>
@@ -8748,7 +8747,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="91" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>110</v>
       </c>
@@ -8813,7 +8812,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="92" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>111</v>
       </c>
@@ -8878,7 +8877,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="93" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>112</v>
       </c>
@@ -8943,7 +8942,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="94" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>113</v>
       </c>
@@ -9008,7 +9007,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="95" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>114</v>
       </c>
@@ -9073,7 +9072,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="96" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>115</v>
       </c>
@@ -9138,7 +9137,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="97" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>116</v>
       </c>
@@ -9203,7 +9202,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="98" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>117</v>
       </c>
@@ -9268,7 +9267,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="99" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>118</v>
       </c>
@@ -9333,7 +9332,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="100" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>119</v>
       </c>
@@ -9398,7 +9397,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="101" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>120</v>
       </c>
@@ -9463,7 +9462,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="102" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>121</v>
       </c>
@@ -9528,7 +9527,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="103" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>122</v>
       </c>
@@ -9593,7 +9592,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="104" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>123</v>
       </c>
@@ -9658,7 +9657,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="105" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>124</v>
       </c>
@@ -9723,7 +9722,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="106" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>125</v>
       </c>
@@ -9788,7 +9787,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="107" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>126</v>
       </c>
@@ -9853,7 +9852,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="108" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>127</v>
       </c>
@@ -9918,7 +9917,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="109" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>128</v>
       </c>
@@ -9983,7 +9982,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="110" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>129</v>
       </c>
@@ -10048,7 +10047,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="111" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>130</v>
       </c>
@@ -10113,7 +10112,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="112" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>131</v>
       </c>
@@ -10178,7 +10177,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="113" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>132</v>
       </c>
@@ -10243,7 +10242,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="114" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>133</v>
       </c>
@@ -10308,7 +10307,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="115" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>134</v>
       </c>
@@ -10373,7 +10372,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="116" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>135</v>
       </c>
@@ -10438,7 +10437,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="117" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>136</v>
       </c>
@@ -10503,7 +10502,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="118" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>137</v>
       </c>
@@ -10568,7 +10567,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="119" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>138</v>
       </c>
@@ -10633,7 +10632,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="120" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>139</v>
       </c>
@@ -10698,7 +10697,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="121" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>140</v>
       </c>
@@ -10763,7 +10762,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="122" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>141</v>
       </c>
@@ -10828,7 +10827,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="123" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>142</v>
       </c>
@@ -10893,7 +10892,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="124" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>143</v>
       </c>
@@ -10958,7 +10957,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="125" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>144</v>
       </c>
@@ -11023,7 +11022,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="126" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>145</v>
       </c>
@@ -11088,7 +11087,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="127" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>146</v>
       </c>
@@ -11153,7 +11152,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="128" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>147</v>
       </c>
@@ -11218,7 +11217,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="129" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>144</v>
       </c>
@@ -11283,7 +11282,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="130" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>148</v>
       </c>
@@ -11348,7 +11347,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="131" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>100</v>
       </c>
@@ -11413,7 +11412,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="132" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>101</v>
       </c>
@@ -11478,7 +11477,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="133" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>102</v>
       </c>
@@ -11543,7 +11542,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="134" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>103</v>
       </c>
@@ -11608,7 +11607,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="135" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>149</v>
       </c>
@@ -11673,7 +11672,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="136" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>150</v>
       </c>
@@ -11738,7 +11737,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="137" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>151</v>
       </c>
@@ -11803,7 +11802,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="138" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>152</v>
       </c>
@@ -11868,7 +11867,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="139" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>153</v>
       </c>
@@ -11933,7 +11932,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="140" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>154</v>
       </c>
@@ -11998,7 +11997,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="141" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>155</v>
       </c>
@@ -12063,7 +12062,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="142" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>156</v>
       </c>
@@ -12128,7 +12127,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="143" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>157</v>
       </c>
@@ -12193,7 +12192,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="144" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>158</v>
       </c>
@@ -12258,7 +12257,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="145" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>159</v>
       </c>
@@ -12323,7 +12322,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="146" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>160</v>
       </c>
@@ -12388,7 +12387,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="147" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>161</v>
       </c>
@@ -12453,7 +12452,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="148" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A148" t="s">
         <v>162</v>
       </c>
@@ -12518,7 +12517,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="149" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>163</v>
       </c>
@@ -12583,7 +12582,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="150" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>164</v>
       </c>
@@ -12648,7 +12647,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="151" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>165</v>
       </c>
@@ -12713,7 +12712,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="152" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>166</v>
       </c>
@@ -12778,7 +12777,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="153" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>167</v>
       </c>
@@ -12843,7 +12842,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="154" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>168</v>
       </c>
@@ -12908,7 +12907,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="155" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>169</v>
       </c>
@@ -12973,7 +12972,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="156" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>170</v>
       </c>
@@ -13038,7 +13037,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="157" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>171</v>
       </c>
@@ -13103,7 +13102,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="158" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>172</v>
       </c>
@@ -13168,7 +13167,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="159" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>173</v>
       </c>
@@ -13233,7 +13232,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="160" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>174</v>
       </c>
@@ -13298,7 +13297,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="161" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>175</v>
       </c>
@@ -13363,7 +13362,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="162" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>176</v>
       </c>
@@ -13428,7 +13427,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="163" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>177</v>
       </c>
@@ -13493,7 +13492,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="164" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>178</v>
       </c>
@@ -13558,7 +13557,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="165" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>179</v>
       </c>
@@ -13623,7 +13622,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="166" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>180</v>
       </c>
@@ -13688,7 +13687,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="167" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>181</v>
       </c>
@@ -13753,7 +13752,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="168" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>182</v>
       </c>
@@ -13818,7 +13817,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="169" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A169" t="s">
         <v>183</v>
       </c>
@@ -13883,7 +13882,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="170" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>184</v>
       </c>
@@ -13948,7 +13947,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="171" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>185</v>
       </c>
@@ -14013,7 +14012,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="172" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A172" t="s">
         <v>186</v>
       </c>
@@ -14078,7 +14077,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="173" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A173" t="s">
         <v>187</v>
       </c>
@@ -14143,7 +14142,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="174" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A174" t="s">
         <v>188</v>
       </c>
@@ -14208,7 +14207,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="175" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A175" t="s">
         <v>189</v>
       </c>
@@ -14273,7 +14272,7 @@
         <v>798</v>
       </c>
     </row>
-    <row r="176" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A176" t="s">
         <v>190</v>
       </c>
@@ -14338,7 +14337,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="177" spans="1:21" hidden="1" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A177" t="s">
         <v>191</v>
       </c>
@@ -14404,15 +14403,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:U177">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="BTS409L1 E3062A"/>
-        <filter val="BTS40K2-1EJC"/>
-        <filter val="BTS40K2-1ENC"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:U177"/>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B3" r:id="rId2"/>

</xml_diff>